<commit_message>
Finished benchmarking. Some final edits.
</commit_message>
<xml_diff>
--- a/testing/comparison_with_matlab.xlsx
+++ b/testing/comparison_with_matlab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\PhD_programs\pyLUKAD\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402F1B5D-E919-45EB-91C4-D690C812A7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF39842-CB64-4A27-A8D0-E479B6865449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{46B94CEE-8924-458A-8CB3-8BAED2345B19}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="22720" windowHeight="14600" xr2:uid="{46B94CEE-8924-458A-8CB3-8BAED2345B19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Software</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Stream time [s]</t>
+  </si>
+  <si>
+    <t>simple_ramp_100x3000</t>
   </si>
 </sst>
 </file>
@@ -102,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +130,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -231,170 +240,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -408,19 +258,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,16 +267,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -756,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F660A277-12DD-49BB-ADA2-74AF5CE12790}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -771,29 +607,29 @@
     <col min="10" max="10" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -807,29 +643,29 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="13">
         <v>1.67</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="13">
         <f>E2-C2</f>
         <v>2.63</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="13">
         <v>4.3</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="13">
         <v>1.64</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="13">
         <v>31.2</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="18"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5" t="s">
         <v>11</v>
@@ -839,29 +675,33 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="13">
         <v>2.35</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="13">
         <v>0.45</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="13">
         <f>D3+C3</f>
         <v>2.8000000000000003</v>
       </c>
-      <c r="F3" s="24">
-        <v>1.73</v>
-      </c>
-      <c r="G3" s="24">
-        <v>33.1</v>
-      </c>
-      <c r="H3" s="17"/>
+      <c r="F3" s="13">
+        <v>1.76</v>
+      </c>
+      <c r="G3" s="13">
+        <v>33.4</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3">
+        <f>G2/G3</f>
+        <v>0.93413173652694614</v>
+      </c>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
         <v>12</v>
@@ -871,108 +711,170 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="14">
         <v>10.6</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="14">
         <f>E4-C4</f>
         <v>5.2000000000000011</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="14">
         <v>15.8</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="14">
         <v>0.53</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="14">
         <v>109</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="14">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="14">
         <v>5.3</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="14">
         <f>D5+C5</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="F5" s="25">
-        <v>0.52</v>
-      </c>
-      <c r="G5" s="25">
-        <v>110</v>
-      </c>
-      <c r="H5" s="17" t="s">
+      <c r="F5" s="14">
+        <v>0.42</v>
+      </c>
+      <c r="G5" s="14">
+        <v>104</v>
+      </c>
+      <c r="H5" s="18" t="s">
         <v>7</v>
+      </c>
+      <c r="I5">
+        <f>G4/G5</f>
+        <v>1.0480769230769231</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="15">
         <v>136</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="15">
         <f>E6-C6</f>
         <v>67</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="15">
         <v>203</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="15">
         <v>0.2</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="15">
         <v>7930</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="15">
         <v>45</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="15">
         <v>329</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="15">
         <f>C7+D7</f>
         <v>374</v>
       </c>
-      <c r="F7" s="27">
-        <v>0.26</v>
-      </c>
-      <c r="G7" s="27">
-        <v>8081</v>
-      </c>
-      <c r="H7" s="22"/>
+      <c r="F7" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G7" s="15">
+        <v>7423</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7">
+        <f>G6/G7</f>
+        <v>1.0683012259194395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="20">
+        <v>2.9</v>
+      </c>
+      <c r="D8" s="16">
+        <f>E8-C8</f>
+        <v>7.2999999999999989</v>
+      </c>
+      <c r="E8" s="20">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F8" s="20">
+        <v>1.06</v>
+      </c>
+      <c r="G8" s="20">
+        <v>177</v>
+      </c>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="20">
+        <v>4.8</v>
+      </c>
+      <c r="D9" s="20">
+        <v>12</v>
+      </c>
+      <c r="E9" s="16">
+        <f>C9+D9</f>
+        <v>16.8</v>
+      </c>
+      <c r="F9" s="20">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
+        <v>171</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9">
+        <f>G8/G9</f>
+        <v>1.0350877192982457</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated building the docs
</commit_message>
<xml_diff>
--- a/testing/comparison_with_matlab.xlsx
+++ b/testing/comparison_with_matlab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\PhD_programs\pyLUKAD\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF39842-CB64-4A27-A8D0-E479B6865449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF5261-DA3E-4A22-A81C-FD508CB41330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="22720" windowHeight="14600" xr2:uid="{46B94CEE-8924-458A-8CB3-8BAED2345B19}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{46B94CEE-8924-458A-8CB3-8BAED2345B19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F660A277-12DD-49BB-ADA2-74AF5CE12790}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -876,6 +876,54 @@
         <v>1.0350877192982457</v>
       </c>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <f>G2/E2</f>
+        <v>7.2558139534883725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <f t="shared" ref="J15:J23" si="0">G3/E3</f>
+        <v>11.928571428571427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>6.8987341772151893</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>10.721649484536083</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>39.064039408866996</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>19.847593582887701</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>17.352941176470591</v>
+      </c>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>10.178571428571429</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>